<commit_message>
file fixes and calculations
</commit_message>
<xml_diff>
--- a/Data/fracstrpanels.xlsx
+++ b/Data/fracstrpanels.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjones/Documents/woodcarb/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24816"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="4020" windowWidth="26680" windowHeight="13200" tabRatio="500"/>
+    <workbookView xWindow="6200" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -113,7 +108,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -148,7 +143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,7 +320,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -333,15 +328,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R151"/>
+  <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1">
         <v>0.37</v>
       </c>
@@ -393,11 +388,8 @@
       <c r="Q1">
         <v>0</v>
       </c>
-      <c r="R1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>0.36994472789115646</v>
       </c>
@@ -449,11 +441,8 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>0.36988945578231291</v>
       </c>
@@ -505,11 +494,8 @@
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>0.36983418367346937</v>
       </c>
@@ -561,11 +547,8 @@
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>0.36977891156462583</v>
       </c>
@@ -617,11 +600,8 @@
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>0.36972363945578229</v>
       </c>
@@ -673,11 +653,8 @@
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>0.36966836734693875</v>
       </c>
@@ -729,11 +706,8 @@
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>0.36961309523809521</v>
       </c>
@@ -785,11 +759,8 @@
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>0.36955782312925167</v>
       </c>
@@ -841,11 +812,8 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>0.36950255102040813</v>
       </c>
@@ -897,11 +865,8 @@
       <c r="Q10">
         <v>0</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>0.36944727891156459</v>
       </c>
@@ -953,11 +918,8 @@
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>0.36939200680272105</v>
       </c>
@@ -1009,11 +971,8 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>0.36933673469387751</v>
       </c>
@@ -1065,11 +1024,8 @@
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>0.36928146258503397</v>
       </c>
@@ -1121,11 +1077,8 @@
       <c r="Q14">
         <v>0</v>
       </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>0.36922619047619043</v>
       </c>
@@ -1177,11 +1130,8 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>0.36917091836734689</v>
       </c>
@@ -1233,11 +1183,8 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>0.36911564625850335</v>
       </c>
@@ -1289,11 +1236,8 @@
       <c r="Q17">
         <v>0</v>
       </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>0.36906037414965981</v>
       </c>
@@ -1345,11 +1289,8 @@
       <c r="Q18">
         <v>0</v>
       </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>0.36900510204081627</v>
       </c>
@@ -1401,11 +1342,8 @@
       <c r="Q19">
         <v>0</v>
       </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>0.36894982993197273</v>
       </c>
@@ -1457,11 +1395,8 @@
       <c r="Q20">
         <v>0</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>0.36889455782312919</v>
       </c>
@@ -1513,11 +1448,8 @@
       <c r="Q21">
         <v>0</v>
       </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>0.36883928571428565</v>
       </c>
@@ -1569,11 +1501,8 @@
       <c r="Q22">
         <v>0</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>0.36878401360544211</v>
       </c>
@@ -1625,11 +1554,8 @@
       <c r="Q23">
         <v>0</v>
       </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>0.36872874149659857</v>
       </c>
@@ -1681,11 +1607,8 @@
       <c r="Q24">
         <v>0</v>
       </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>0.36867346938775503</v>
       </c>
@@ -1737,11 +1660,8 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>0.36861819727891149</v>
       </c>
@@ -1793,11 +1713,8 @@
       <c r="Q26">
         <v>0</v>
       </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>0.36856292517006795</v>
       </c>
@@ -1849,11 +1766,8 @@
       <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>0.36850765306122441</v>
       </c>
@@ -1905,11 +1819,8 @@
       <c r="Q28">
         <v>0</v>
       </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>0.36845238095238086</v>
       </c>
@@ -1961,11 +1872,8 @@
       <c r="Q29">
         <v>0</v>
       </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>0.36839710884353732</v>
       </c>
@@ -2017,11 +1925,8 @@
       <c r="Q30">
         <v>0</v>
       </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>0.36834183673469378</v>
       </c>
@@ -2073,11 +1978,8 @@
       <c r="Q31">
         <v>0</v>
       </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>0.36828656462585024</v>
       </c>
@@ -2129,11 +2031,8 @@
       <c r="Q32">
         <v>0</v>
       </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>0.3682312925170067</v>
       </c>
@@ -2185,11 +2084,8 @@
       <c r="Q33">
         <v>0</v>
       </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>0.36817602040816316</v>
       </c>
@@ -2241,11 +2137,8 @@
       <c r="Q34">
         <v>0</v>
       </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>0.36812074829931962</v>
       </c>
@@ -2297,11 +2190,8 @@
       <c r="Q35">
         <v>0</v>
       </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>0.36806547619047608</v>
       </c>
@@ -2353,11 +2243,8 @@
       <c r="Q36">
         <v>0</v>
       </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>0.36801020408163254</v>
       </c>
@@ -2409,11 +2296,8 @@
       <c r="Q37">
         <v>0</v>
       </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>0.367954931972789</v>
       </c>
@@ -2465,11 +2349,8 @@
       <c r="Q38">
         <v>0</v>
       </c>
-      <c r="R38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>0.36789965986394546</v>
       </c>
@@ -2521,11 +2402,8 @@
       <c r="Q39">
         <v>0</v>
       </c>
-      <c r="R39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>0.36784438775510192</v>
       </c>
@@ -2577,11 +2455,8 @@
       <c r="Q40">
         <v>0</v>
       </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>0.36778911564625838</v>
       </c>
@@ -2633,11 +2508,8 @@
       <c r="Q41">
         <v>0</v>
       </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>0.36773384353741484</v>
       </c>
@@ -2689,11 +2561,8 @@
       <c r="Q42">
         <v>0</v>
       </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>0.3676785714285713</v>
       </c>
@@ -2745,11 +2614,8 @@
       <c r="Q43">
         <v>0</v>
       </c>
-      <c r="R43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>0.36762329931972776</v>
       </c>
@@ -2801,11 +2667,8 @@
       <c r="Q44">
         <v>0</v>
       </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>0.36756802721088422</v>
       </c>
@@ -2857,11 +2720,8 @@
       <c r="Q45">
         <v>0</v>
       </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>0.36751275510204068</v>
       </c>
@@ -2913,11 +2773,8 @@
       <c r="Q46">
         <v>0</v>
       </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>0.36745748299319714</v>
       </c>
@@ -2969,11 +2826,8 @@
       <c r="Q47">
         <v>0</v>
       </c>
-      <c r="R47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>0.3674022108843536</v>
       </c>
@@ -3025,11 +2879,8 @@
       <c r="Q48">
         <v>0</v>
       </c>
-      <c r="R48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>0.36734693877551017</v>
       </c>
@@ -3081,11 +2932,8 @@
       <c r="Q49">
         <v>0</v>
       </c>
-      <c r="R49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>0.36253644314868799</v>
       </c>
@@ -3137,11 +2985,8 @@
       <c r="Q50">
         <v>0</v>
       </c>
-      <c r="R50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>0.35772594752186582</v>
       </c>
@@ -3193,11 +3038,8 @@
       <c r="Q51">
         <v>0</v>
       </c>
-      <c r="R51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>0.35291545189504364</v>
       </c>
@@ -3249,11 +3091,8 @@
       <c r="Q52">
         <v>0</v>
       </c>
-      <c r="R52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>0.34810495626822147</v>
       </c>
@@ -3305,11 +3144,8 @@
       <c r="Q53">
         <v>0</v>
       </c>
-      <c r="R53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54">
         <v>0.34329446064139929</v>
       </c>
@@ -3361,11 +3197,8 @@
       <c r="Q54">
         <v>0</v>
       </c>
-      <c r="R54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55">
         <v>0.33848396501457712</v>
       </c>
@@ -3417,11 +3250,8 @@
       <c r="Q55">
         <v>0</v>
       </c>
-      <c r="R55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56">
         <v>0.33367346938775494</v>
       </c>
@@ -3473,11 +3303,8 @@
       <c r="Q56">
         <v>0</v>
       </c>
-      <c r="R56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57">
         <v>0.32886297376093276</v>
       </c>
@@ -3529,11 +3356,8 @@
       <c r="Q57">
         <v>0</v>
       </c>
-      <c r="R57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58">
         <v>0.32405247813411059</v>
       </c>
@@ -3585,11 +3409,8 @@
       <c r="Q58">
         <v>0</v>
       </c>
-      <c r="R58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59">
         <v>0.31924198250728841</v>
       </c>
@@ -3641,11 +3462,8 @@
       <c r="Q59">
         <v>0</v>
       </c>
-      <c r="R59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60">
         <v>0.31443148688046624</v>
       </c>
@@ -3697,11 +3515,8 @@
       <c r="Q60">
         <v>0</v>
       </c>
-      <c r="R60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61">
         <v>0.30962099125364406</v>
       </c>
@@ -3753,11 +3568,8 @@
       <c r="Q61">
         <v>0</v>
       </c>
-      <c r="R61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62">
         <v>0.30481049562682189</v>
       </c>
@@ -3809,11 +3621,8 @@
       <c r="Q62">
         <v>0</v>
       </c>
-      <c r="R62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63">
         <v>0.3</v>
       </c>
@@ -3865,11 +3674,8 @@
       <c r="Q63">
         <v>0</v>
       </c>
-      <c r="R63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64">
         <v>0.30624999999999997</v>
       </c>
@@ -3921,11 +3727,8 @@
       <c r="Q64">
         <v>0</v>
       </c>
-      <c r="R64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65">
         <v>0.31249999999999994</v>
       </c>
@@ -3977,11 +3780,8 @@
       <c r="Q65">
         <v>0</v>
       </c>
-      <c r="R65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66">
         <v>0.31874999999999992</v>
       </c>
@@ -4033,11 +3833,8 @@
       <c r="Q66">
         <v>0</v>
       </c>
-      <c r="R66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67">
         <v>0.3249999999999999</v>
       </c>
@@ -4089,11 +3886,8 @@
       <c r="Q67">
         <v>0</v>
       </c>
-      <c r="R67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:17">
       <c r="A68">
         <v>0.33124999999999988</v>
       </c>
@@ -4145,11 +3939,8 @@
       <c r="Q68">
         <v>0</v>
       </c>
-      <c r="R68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:17">
       <c r="A69">
         <v>0.33749999999999986</v>
       </c>
@@ -4201,11 +3992,8 @@
       <c r="Q69">
         <v>0</v>
       </c>
-      <c r="R69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:17">
       <c r="A70">
         <v>0.34374999999999983</v>
       </c>
@@ -4257,11 +4045,8 @@
       <c r="Q70">
         <v>0</v>
       </c>
-      <c r="R70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:17">
       <c r="A71">
         <v>0.34999999999999981</v>
       </c>
@@ -4313,11 +4098,8 @@
       <c r="Q71">
         <v>0</v>
       </c>
-      <c r="R71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:17">
       <c r="A72">
         <v>0.35624999999999979</v>
       </c>
@@ -4369,11 +4151,8 @@
       <c r="Q72">
         <v>0</v>
       </c>
-      <c r="R72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:17">
       <c r="A73">
         <v>0.36249999999999977</v>
       </c>
@@ -4425,11 +4204,8 @@
       <c r="Q73">
         <v>0</v>
       </c>
-      <c r="R73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:17">
       <c r="A74">
         <v>0.36874999999999974</v>
       </c>
@@ -4481,11 +4257,8 @@
       <c r="Q74">
         <v>0</v>
       </c>
-      <c r="R74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:17">
       <c r="A75">
         <v>0.37499999999999972</v>
       </c>
@@ -4537,11 +4310,8 @@
       <c r="Q75">
         <v>0</v>
       </c>
-      <c r="R75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:17">
       <c r="A76">
         <v>0.3812499999999997</v>
       </c>
@@ -4593,11 +4363,8 @@
       <c r="Q76">
         <v>0</v>
       </c>
-      <c r="R76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:17">
       <c r="A77">
         <v>0.38749999999999968</v>
       </c>
@@ -4649,11 +4416,8 @@
       <c r="Q77">
         <v>0</v>
       </c>
-      <c r="R77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78">
         <v>0.39374999999999966</v>
       </c>
@@ -4705,11 +4469,8 @@
       <c r="Q78">
         <v>0</v>
       </c>
-      <c r="R78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:17">
       <c r="A79">
         <v>0.39999999999999963</v>
       </c>
@@ -4761,11 +4522,8 @@
       <c r="Q79">
         <v>0</v>
       </c>
-      <c r="R79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:17">
       <c r="A80">
         <v>0.40624999999999961</v>
       </c>
@@ -4817,11 +4575,8 @@
       <c r="Q80">
         <v>0</v>
       </c>
-      <c r="R80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:17">
       <c r="A81">
         <v>0.41249999999999959</v>
       </c>
@@ -4873,11 +4628,8 @@
       <c r="Q81">
         <v>0</v>
       </c>
-      <c r="R81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:17">
       <c r="A82">
         <v>0.41874999999999957</v>
       </c>
@@ -4929,11 +4681,8 @@
       <c r="Q82">
         <v>0</v>
       </c>
-      <c r="R82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:17">
       <c r="A83">
         <v>0.42499999999999954</v>
       </c>
@@ -4985,11 +4734,8 @@
       <c r="Q83">
         <v>0</v>
       </c>
-      <c r="R83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84">
         <v>0.43124999999999952</v>
       </c>
@@ -5041,11 +4787,8 @@
       <c r="Q84">
         <v>0</v>
       </c>
-      <c r="R84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:17">
       <c r="A85">
         <v>0.4374999999999995</v>
       </c>
@@ -5097,11 +4840,8 @@
       <c r="Q85">
         <v>0</v>
       </c>
-      <c r="R85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:17">
       <c r="A86">
         <v>0.44374999999999948</v>
       </c>
@@ -5153,11 +4893,8 @@
       <c r="Q86">
         <v>0</v>
       </c>
-      <c r="R86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:17">
       <c r="A87">
         <v>0.45</v>
       </c>
@@ -5209,11 +4946,8 @@
       <c r="Q87">
         <v>0</v>
       </c>
-      <c r="R87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88">
         <v>0.45147891133561818</v>
       </c>
@@ -5265,11 +4999,8 @@
       <c r="Q88">
         <v>0</v>
       </c>
-      <c r="R88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:17">
       <c r="A89">
         <v>0.45295782267123635</v>
       </c>
@@ -5321,11 +5052,8 @@
       <c r="Q89">
         <v>0</v>
       </c>
-      <c r="R89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:17">
       <c r="A90">
         <v>0.45443673400685453</v>
       </c>
@@ -5377,11 +5105,8 @@
       <c r="Q90">
         <v>0</v>
       </c>
-      <c r="R90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:17">
       <c r="A91">
         <v>0.4559156453424727</v>
       </c>
@@ -5433,11 +5158,8 @@
       <c r="Q91">
         <v>0</v>
       </c>
-      <c r="R91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:17">
       <c r="A92">
         <v>0.45739455667809087</v>
       </c>
@@ -5489,11 +5211,8 @@
       <c r="Q92">
         <v>0</v>
       </c>
-      <c r="R92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:17">
       <c r="A93">
         <v>0.45887346801370904</v>
       </c>
@@ -5545,11 +5264,8 @@
       <c r="Q93">
         <v>0</v>
       </c>
-      <c r="R93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:17">
       <c r="A94">
         <v>0.46035237934932721</v>
       </c>
@@ -5601,11 +5317,8 @@
       <c r="Q94">
         <v>0</v>
       </c>
-      <c r="R94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:17">
       <c r="A95">
         <v>0.46183129068494538</v>
       </c>
@@ -5657,11 +5370,8 @@
       <c r="Q95">
         <v>0</v>
       </c>
-      <c r="R95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:17">
       <c r="A96">
         <v>0.46331020202056356</v>
       </c>
@@ -5713,11 +5423,8 @@
       <c r="Q96">
         <v>0</v>
       </c>
-      <c r="R96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:17">
       <c r="A97">
         <v>0.46478911335618173</v>
       </c>
@@ -5769,11 +5476,8 @@
       <c r="Q97">
         <v>0</v>
       </c>
-      <c r="R97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:17">
       <c r="A98">
         <v>0.4662680246917999</v>
       </c>
@@ -5825,11 +5529,8 @@
       <c r="Q98">
         <v>0</v>
       </c>
-      <c r="R98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:17">
       <c r="A99">
         <v>0.46774693602741818</v>
       </c>
@@ -5881,11 +5582,8 @@
       <c r="Q99">
         <v>0</v>
       </c>
-      <c r="R99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:17">
       <c r="A100">
         <v>0.46774693602741818</v>
       </c>
@@ -5937,11 +5635,8 @@
       <c r="Q100">
         <v>0</v>
       </c>
-      <c r="R100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:17">
       <c r="A101">
         <v>0.46774693602741818</v>
       </c>
@@ -5993,11 +5688,8 @@
       <c r="Q101">
         <v>0</v>
       </c>
-      <c r="R101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:17">
       <c r="A102">
         <v>0.46774693602741818</v>
       </c>
@@ -6049,11 +5741,8 @@
       <c r="Q102">
         <v>0</v>
       </c>
-      <c r="R102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:17">
       <c r="A103">
         <v>0.46774693602741818</v>
       </c>
@@ -6105,11 +5794,8 @@
       <c r="Q103">
         <v>0</v>
       </c>
-      <c r="R103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:17">
       <c r="A104">
         <v>0.46774693602741818</v>
       </c>
@@ -6161,11 +5847,8 @@
       <c r="Q104">
         <v>0</v>
       </c>
-      <c r="R104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:17">
       <c r="A105">
         <v>0.46774693602741818</v>
       </c>
@@ -6217,11 +5900,8 @@
       <c r="Q105">
         <v>0</v>
       </c>
-      <c r="R105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:17">
       <c r="A106">
         <v>0.46774693602741818</v>
       </c>
@@ -6273,11 +5953,8 @@
       <c r="Q106">
         <v>0</v>
       </c>
-      <c r="R106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:17">
       <c r="A107">
         <v>0.46774693602741818</v>
       </c>
@@ -6329,11 +6006,8 @@
       <c r="Q107">
         <v>0</v>
       </c>
-      <c r="R107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:17">
       <c r="A108">
         <v>0.46774693602741818</v>
       </c>
@@ -6385,11 +6059,8 @@
       <c r="Q108">
         <v>0</v>
       </c>
-      <c r="R108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:17">
       <c r="A109">
         <v>0.46774693602741818</v>
       </c>
@@ -6441,11 +6112,8 @@
       <c r="Q109">
         <v>0</v>
       </c>
-      <c r="R109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:17">
       <c r="A110">
         <v>0.46774693602741818</v>
       </c>
@@ -6497,11 +6165,8 @@
       <c r="Q110">
         <v>0</v>
       </c>
-      <c r="R110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:17">
       <c r="A111">
         <v>0.46774693602741818</v>
       </c>
@@ -6553,11 +6218,8 @@
       <c r="Q111">
         <v>0</v>
       </c>
-      <c r="R111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:17">
       <c r="A112">
         <v>0.46774693602741818</v>
       </c>
@@ -6609,11 +6271,8 @@
       <c r="Q112">
         <v>0</v>
       </c>
-      <c r="R112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:17">
       <c r="A113">
         <v>0.46774693602741818</v>
       </c>
@@ -6665,11 +6324,8 @@
       <c r="Q113">
         <v>0</v>
       </c>
-      <c r="R113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:17">
       <c r="A114">
         <v>0.46774693602741818</v>
       </c>
@@ -6721,11 +6377,8 @@
       <c r="Q114">
         <v>0</v>
       </c>
-      <c r="R114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:17">
       <c r="A115">
         <v>0.46774693602741818</v>
       </c>
@@ -6777,11 +6430,8 @@
       <c r="Q115">
         <v>0</v>
       </c>
-      <c r="R115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:17">
       <c r="A116">
         <v>0.46774693602741818</v>
       </c>
@@ -6833,11 +6483,8 @@
       <c r="Q116">
         <v>0</v>
       </c>
-      <c r="R116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117">
         <v>0.46774693602741818</v>
       </c>
@@ -6889,11 +6536,8 @@
       <c r="Q117">
         <v>0</v>
       </c>
-      <c r="R117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:17">
       <c r="A118">
         <v>0.46774693602741818</v>
       </c>
@@ -6945,11 +6589,8 @@
       <c r="Q118">
         <v>0</v>
       </c>
-      <c r="R118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:17">
       <c r="A119">
         <v>0.46774693602741818</v>
       </c>
@@ -7001,11 +6642,8 @@
       <c r="Q119">
         <v>0</v>
       </c>
-      <c r="R119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120">
         <v>0.46774693602741818</v>
       </c>
@@ -7057,11 +6695,8 @@
       <c r="Q120">
         <v>0</v>
       </c>
-      <c r="R120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:17">
       <c r="A121">
         <v>0.46774693602741818</v>
       </c>
@@ -7113,11 +6748,8 @@
       <c r="Q121">
         <v>0</v>
       </c>
-      <c r="R121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:17">
       <c r="A122">
         <v>0.46774693602741818</v>
       </c>
@@ -7169,11 +6801,8 @@
       <c r="Q122">
         <v>0</v>
       </c>
-      <c r="R122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:17">
       <c r="A123">
         <v>0.46774693602741818</v>
       </c>
@@ -7225,11 +6854,8 @@
       <c r="Q123">
         <v>0</v>
       </c>
-      <c r="R123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:17">
       <c r="A124">
         <v>0.46774693602741818</v>
       </c>
@@ -7281,11 +6907,8 @@
       <c r="Q124">
         <v>0</v>
       </c>
-      <c r="R124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:17">
       <c r="A125">
         <v>0.46774693602741818</v>
       </c>
@@ -7337,11 +6960,8 @@
       <c r="Q125">
         <v>0</v>
       </c>
-      <c r="R125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:17">
       <c r="A126">
         <v>0.46774693602741818</v>
       </c>
@@ -7393,11 +7013,8 @@
       <c r="Q126">
         <v>0</v>
       </c>
-      <c r="R126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:17">
       <c r="A127">
         <v>0.46774693602741818</v>
       </c>
@@ -7449,11 +7066,8 @@
       <c r="Q127">
         <v>0</v>
       </c>
-      <c r="R127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:17">
       <c r="A128">
         <v>0.46774693602741818</v>
       </c>
@@ -7505,11 +7119,8 @@
       <c r="Q128">
         <v>0</v>
       </c>
-      <c r="R128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:17">
       <c r="A129">
         <v>0.46774693602741818</v>
       </c>
@@ -7561,11 +7172,8 @@
       <c r="Q129">
         <v>0</v>
       </c>
-      <c r="R129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:17">
       <c r="A130">
         <v>0.46774693602741818</v>
       </c>
@@ -7617,11 +7225,8 @@
       <c r="Q130">
         <v>0</v>
       </c>
-      <c r="R130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:17">
       <c r="A131">
         <v>0.46774693602741818</v>
       </c>
@@ -7673,11 +7278,8 @@
       <c r="Q131">
         <v>0</v>
       </c>
-      <c r="R131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132">
         <v>0.46774693602741818</v>
       </c>
@@ -7729,11 +7331,8 @@
       <c r="Q132">
         <v>0</v>
       </c>
-      <c r="R132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:17">
       <c r="A133">
         <v>0.46774693602741818</v>
       </c>
@@ -7785,11 +7384,8 @@
       <c r="Q133">
         <v>0</v>
       </c>
-      <c r="R133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:17">
       <c r="A134">
         <v>0.46774693602741818</v>
       </c>
@@ -7841,11 +7437,8 @@
       <c r="Q134">
         <v>0</v>
       </c>
-      <c r="R134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:17">
       <c r="A135">
         <v>0.46774693602741818</v>
       </c>
@@ -7897,11 +7490,8 @@
       <c r="Q135">
         <v>0</v>
       </c>
-      <c r="R135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:17">
       <c r="A136">
         <v>0.46774693602741818</v>
       </c>
@@ -7953,11 +7543,8 @@
       <c r="Q136">
         <v>0</v>
       </c>
-      <c r="R136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:17">
       <c r="A137">
         <v>0.46774693602741818</v>
       </c>
@@ -8009,11 +7596,8 @@
       <c r="Q137">
         <v>0</v>
       </c>
-      <c r="R137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:17">
       <c r="A138">
         <v>0.46774693602741818</v>
       </c>
@@ -8065,11 +7649,8 @@
       <c r="Q138">
         <v>0</v>
       </c>
-      <c r="R138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:17">
       <c r="A139">
         <v>0.46774693602741818</v>
       </c>
@@ -8121,11 +7702,8 @@
       <c r="Q139">
         <v>0</v>
       </c>
-      <c r="R139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:17">
       <c r="A140">
         <v>0.46774693602741818</v>
       </c>
@@ -8177,11 +7755,8 @@
       <c r="Q140">
         <v>0</v>
       </c>
-      <c r="R140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:17">
       <c r="A141">
         <v>0.46774693602741818</v>
       </c>
@@ -8233,11 +7808,8 @@
       <c r="Q141">
         <v>0</v>
       </c>
-      <c r="R141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:17">
       <c r="A142">
         <v>0.46774693602741818</v>
       </c>
@@ -8289,11 +7861,8 @@
       <c r="Q142">
         <v>0</v>
       </c>
-      <c r="R142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:17">
       <c r="A143">
         <v>0.46774693602741818</v>
       </c>
@@ -8345,11 +7914,8 @@
       <c r="Q143">
         <v>0</v>
       </c>
-      <c r="R143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:17">
       <c r="A144">
         <v>0.46774693602741818</v>
       </c>
@@ -8401,11 +7967,8 @@
       <c r="Q144">
         <v>0</v>
       </c>
-      <c r="R144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:17">
       <c r="A145">
         <v>0.46774693602741818</v>
       </c>
@@ -8457,11 +8020,8 @@
       <c r="Q145">
         <v>0</v>
       </c>
-      <c r="R145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:17">
       <c r="A146">
         <v>0.46774693602741818</v>
       </c>
@@ -8513,11 +8073,8 @@
       <c r="Q146">
         <v>0</v>
       </c>
-      <c r="R146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:17">
       <c r="A147">
         <v>0.46774693602741818</v>
       </c>
@@ -8569,11 +8126,8 @@
       <c r="Q147">
         <v>0</v>
       </c>
-      <c r="R147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:17">
       <c r="A148">
         <v>0.46774693602741818</v>
       </c>
@@ -8625,11 +8179,8 @@
       <c r="Q148">
         <v>0</v>
       </c>
-      <c r="R148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:17">
       <c r="A149">
         <v>0.46774693602741818</v>
       </c>
@@ -8681,11 +8232,8 @@
       <c r="Q149">
         <v>0</v>
       </c>
-      <c r="R149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:17">
       <c r="A150">
         <v>0.46774693602741818</v>
       </c>
@@ -8737,11 +8285,8 @@
       <c r="Q150">
         <v>0</v>
       </c>
-      <c r="R150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:17">
       <c r="A151">
         <v>0.46774693602741818</v>
       </c>
@@ -8791,14 +8336,16 @@
         <v>0</v>
       </c>
       <c r="Q151">
-        <v>0</v>
-      </c>
-      <c r="R151">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>